<commit_message>
Add M7 and COM events.
</commit_message>
<xml_diff>
--- a/2020/com-20200712.xlsx
+++ b/2020/com-20200712.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrye/personal/mac/results/2020/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E93941-6085-964F-A144-BD557A272C08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6315" yWindow="-30" windowWidth="15060" windowHeight="7650"/>
+    <workbookView xWindow="6320" yWindow="460" windowWidth="15060" windowHeight="7660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -84,9 +90,6 @@
     <t xml:space="preserve"> DAN NIELSEN</t>
   </si>
   <si>
-    <t xml:space="preserve"> JAN HANNA</t>
-  </si>
-  <si>
     <t xml:space="preserve"> SHAWN HANNA</t>
   </si>
   <si>
@@ -394,13 +397,16 @@
   </si>
   <si>
     <t xml:space="preserve"> 0:51.830</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JANET HANNA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -722,30 +728,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -762,73 +768,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -836,186 +842,186 @@
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="3" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="3" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="3" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="3" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
-      <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
-      <c r="B25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="3" t="s">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
-      <c r="B27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>19</v>
       </c>
@@ -1023,21 +1029,21 @@
         <v>16</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
-      <c r="B33" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>14</v>
       </c>
@@ -1045,65 +1051,65 @@
         <v>13</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>14</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="B38" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
-      <c r="B41" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41" s="3" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
-      <c r="B42" t="s">
-        <v>30</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>18</v>
       </c>
@@ -1111,23 +1117,23 @@
         <v>7</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
-      <c r="B46" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B48" t="s">
         <v>12</v>
@@ -1136,68 +1142,68 @@
         <v>9</v>
       </c>
       <c r="E48" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B49" t="s">
         <v>12</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E49" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
-      <c r="A50" t="s">
-        <v>36</v>
-      </c>
-      <c r="B50" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>35</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E50" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" t="s">
-        <v>36</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E52" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
-      <c r="A52" t="s">
-        <v>36</v>
-      </c>
-      <c r="B52" t="s">
-        <v>45</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E52" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B53" t="s">
         <v>14</v>
@@ -1206,147 +1212,147 @@
         <v>10</v>
       </c>
       <c r="E53" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" t="s">
+        <v>34</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E54" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
-      <c r="A54" t="s">
-        <v>36</v>
-      </c>
-      <c r="B54" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>35</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E54" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" t="s">
-        <v>36</v>
       </c>
       <c r="B55" t="s">
         <v>18</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E55" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B56" t="s">
         <v>12</v>
       </c>
       <c r="C56" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E56" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" t="s">
+        <v>46</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E57" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
-      <c r="A57" t="s">
-        <v>36</v>
-      </c>
-      <c r="B57" t="s">
-        <v>47</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E57" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B58" t="s">
         <v>17</v>
       </c>
       <c r="C58" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E58" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" t="s">
+        <v>47</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E59" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
-      <c r="A59" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>35</v>
+      </c>
+      <c r="B60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E60" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" t="s">
+        <v>49</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>37</v>
+      </c>
+      <c r="B63" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B59" t="s">
-        <v>48</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E59" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" t="s">
-        <v>36</v>
-      </c>
-      <c r="B60" t="s">
-        <v>49</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E60" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" t="s">
-        <v>36</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="E63" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>37</v>
+      </c>
+      <c r="B64" t="s">
         <v>50</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E61" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" t="s">
-        <v>38</v>
-      </c>
-      <c r="B63" t="s">
-        <v>35</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E63" t="s">
+      <c r="E64" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" t="s">
-        <v>38</v>
-      </c>
-      <c r="B64" t="s">
-        <v>51</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E64" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>